<commit_message>
Fix some wrong files
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Testdata.xlsx
+++ b/src/test/resources/data/Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\demoqa4\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E14BA4-C19C-4E04-A21C-0ACDEB8555E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34DBDA-2018-4357-AF14-DC172C1CE35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{1D695760-1EB8-4935-A17D-5A7E0FAA02CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D695760-1EB8-4935-A17D-5A7E0FAA02CC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>https://demoqa.com/</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>You entered Sara</t>
+  </si>
+  <si>
+    <t>laura.neira@sophos.com</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Neira</t>
   </si>
 </sst>
 </file>
@@ -508,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839E0E08-E5DE-4495-97A4-D2EEBFB382C1}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,13 +593,34 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CDF8CE2C-FB26-46D4-A756-85F8FE3F7894}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{B5325823-F5D4-45F4-AC7A-5C4D775FC5EB}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{FC29B030-38FF-4541-8843-DE34F9C6091C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -627,10 +657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0FA121-1026-44AF-8F12-2CDEA8817937}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,10 +683,16 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{136933C3-978F-42FA-92E3-E7F140232456}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{01B6CEC1-E54A-49F8-BAED-C2B65F580439}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{829C34EA-C5FF-4184-91E5-7C18D27E5553}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -769,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D681808-88F2-46D0-AD28-C9BEC5E2EDAE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>